<commit_message>
Submitted to Nat communications
This commit reflects changes that are current up until our submission
to Nature communications on Oct 5, 2016
</commit_message>
<xml_diff>
--- a/paper/Biswas_et_al_2016_submission/Biswas_2016_Supplemental_Tables.xlsx
+++ b/paper/Biswas_et_al_2016_submission/Biswas_2016_Supplemental_Tables.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16660" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="4440" yWindow="0" windowWidth="20340" windowHeight="16800" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
     <sheet name="Table 3" sheetId="3" r:id="rId3"/>
     <sheet name="Table 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Table 5" sheetId="5" r:id="rId5"/>
-    <sheet name="Table 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Table 5" sheetId="8" r:id="rId5"/>
+    <sheet name="Table 6" sheetId="7" r:id="rId6"/>
+    <sheet name="Table 7" sheetId="5" r:id="rId7"/>
+    <sheet name="Table 8" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="803">
   <si>
     <t>Min GO Term size: 1</t>
   </si>
@@ -2525,12 +2527,79 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">6.9K </t>
+  </si>
+  <si>
+    <t>A. thaliana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110.6K </t>
+  </si>
+  <si>
+    <t>M. musculus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.6K </t>
+  </si>
+  <si>
+    <t>D. melanogaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.7K </t>
+  </si>
+  <si>
+    <t>S. cerevisiae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72.1K </t>
+  </si>
+  <si>
+    <r>
+      <t>H. sapiens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (public)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7K </t>
+  </si>
+  <si>
+    <t>C. elegans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.1K </t>
+  </si>
+  <si>
+    <t>D. Rerio</t>
+  </si>
+  <si>
+    <t>Supplemental Table 5. Number of SRA RNA-Seq records for several model organisms (current as of September 23, 2016)</t>
+  </si>
+  <si>
+    <t>PCC</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>Supplemental Table 6. Test-set PCC for the bottom 20 and top 20 A. thaliana programs when gene-to-program assignments are 100% random.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2588,6 +2657,28 @@
       <color rgb="FF3366FF"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2687,7 +2778,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2733,8 +2824,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2749,8 +2846,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2773,6 +2882,9 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2795,6 +2907,9 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -11338,6 +11453,452 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="14" t="s">
+        <v>784</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="14" t="s">
+        <v>786</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="14" t="s">
+        <v>788</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="14" t="s">
+        <v>790</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="14" t="s">
+        <v>792</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="14" t="s">
+        <v>794</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="14" t="s">
+        <v>796</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>797</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="73.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="16" t="s">
+        <v>799</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="17">
+        <v>0.107</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="17">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="17">
+        <v>0.124</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="17">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="17">
+        <v>0.152</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="17">
+        <v>0.187</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="17">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="17">
+        <v>0.222</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="17">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="17">
+        <v>0.24</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="17">
+        <v>0.247</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="17">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="17">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="17">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="17">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="17">
+        <v>0.308</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="17">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="17">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="17" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="17">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="17">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="17">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="17">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="17">
+        <v>0.94</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="17">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="17">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="17">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="17">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="17">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="17">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="17">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="17">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="17">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="17">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="17">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="17">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="17">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>527</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14311,11 +14872,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>